<commit_message>
Repair xlsx, home and block xlsx for non accepted
</commit_message>
<xml_diff>
--- a/dcrm/website/templates/template_vps.xlsx
+++ b/dcrm/website/templates/template_vps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DS\Desktop\wyceny\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reqsx\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00980655-E513-40C5-88EE-06E5F97B0FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5633A4D-CC11-4999-97E9-23F5FC4EDBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{DBA79AA0-2E99-482A-ABE5-CF2E2EABE4C6}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="16440" windowHeight="28320" firstSheet="1" activeTab="1" xr2:uid="{DBA79AA0-2E99-482A-ABE5-CF2E2EABE4C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Kursy i wyliczenia" sheetId="3" state="hidden" r:id="rId1"/>
@@ -22,10 +22,19 @@
   <definedNames>
     <definedName name="tabela_a" localSheetId="0">'Kursy i wyliczenia'!$A$1:$C$34</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1407,17 +1416,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1457,7 +1466,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1472,7 +1481,7 @@
         <v>81.400000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>89</v>
       </c>
@@ -1483,7 +1492,7 @@
         <v>2.6211000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1504,7 +1513,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -1523,7 +1532,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1538,7 +1547,7 @@
         <v>74.25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1549,7 +1558,7 @@
         <v>2.9819</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -1570,7 +1579,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>103</v>
       </c>
@@ -1589,7 +1598,7 @@
         <v>11.100000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>107</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>4.9960000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>109</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>203.5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -1681,7 +1690,7 @@
         <v>0.58579999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>118</v>
       </c>
@@ -1702,7 +1711,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>121</v>
       </c>
@@ -1721,7 +1730,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -1736,7 +1745,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>0.87870000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -1758,7 +1767,7 @@
         <v>2.2332999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>0.13900000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>131</v>
       </c>
@@ -1780,7 +1789,7 @@
         <v>1.0726</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -1791,7 +1800,7 @@
         <v>0.44950000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>7.2099999999999997E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -1813,7 +1822,7 @@
         <v>0.23280000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>0.2175</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -1835,7 +1844,7 @@
         <v>0.81399999999999995</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>143</v>
       </c>
@@ -1846,7 +1855,7 @@
         <v>0.85570000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>145</v>
       </c>
@@ -1857,7 +1866,7 @@
         <v>2.5859000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>147</v>
       </c>
@@ -1868,7 +1877,7 @@
         <v>4.7915000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -1879,7 +1888,7 @@
         <v>0.30969999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -1890,7 +1899,7 @@
         <v>0.5575</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>153</v>
       </c>
@@ -1918,26 +1927,26 @@
   <dimension ref="A1:V1027"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="7.5546875" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="7.5703125" customWidth="1"/>
     <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="26" width="7.5546875" customWidth="1"/>
+    <col min="14" max="26" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>157</v>
       </c>
@@ -1958,7 +1967,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1969,7 +1978,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="60" t="s">
         <v>32</v>
       </c>
@@ -1982,7 +1991,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -2000,7 +2009,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -2019,7 +2028,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -2038,7 +2047,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="62" t="s">
         <v>38</v>
       </c>
@@ -2057,7 +2066,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="63"/>
       <c r="B8" s="66"/>
       <c r="C8" s="69"/>
@@ -2070,7 +2079,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="64"/>
       <c r="B9" s="67"/>
       <c r="C9" s="70"/>
@@ -2083,16 +2092,14 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="62" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="29">
-        <v>1</v>
-      </c>
+      <c r="C10" s="29"/>
       <c r="D10" s="28" t="s">
         <v>45</v>
       </c>
@@ -2104,7 +2111,7 @@
       <c r="I10" s="31"/>
       <c r="L10" s="31"/>
     </row>
-    <row r="11" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="63"/>
       <c r="B11" s="25" t="s">
         <v>46</v>
@@ -2121,7 +2128,7 @@
       <c r="I11" s="31"/>
       <c r="L11" s="31"/>
     </row>
-    <row r="12" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="64"/>
       <c r="B12" s="25" t="s">
         <v>48</v>
@@ -2138,7 +2145,7 @@
       <c r="I12" s="31"/>
       <c r="L12" s="31"/>
     </row>
-    <row r="13" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>50</v>
       </c>
@@ -2159,7 +2166,7 @@
       <c r="I13" s="31"/>
       <c r="L13" s="31"/>
     </row>
-    <row r="14" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="62" t="s">
         <v>53</v>
       </c>
@@ -2180,7 +2187,7 @@
       <c r="I14" s="31"/>
       <c r="L14" s="31"/>
     </row>
-    <row r="15" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="64"/>
       <c r="B15" s="25" t="s">
         <v>56</v>
@@ -2197,7 +2204,7 @@
       <c r="I15" s="31"/>
       <c r="L15" s="31"/>
     </row>
-    <row r="16" spans="1:13" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2212,7 +2219,7 @@
       <c r="J16" s="31"/>
       <c r="M16" s="31"/>
     </row>
-    <row r="17" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="s">
         <v>6</v>
       </c>
@@ -2227,7 +2234,7 @@
       <c r="M17" s="31"/>
       <c r="P17" s="31"/>
     </row>
-    <row r="18" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
@@ -2246,7 +2253,7 @@
       <c r="J18" s="31"/>
       <c r="M18" s="31"/>
     </row>
-    <row r="19" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>10</v>
       </c>
@@ -2266,7 +2273,7 @@
       <c r="J19" s="31"/>
       <c r="M19" s="31"/>
     </row>
-    <row r="20" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>59</v>
       </c>
@@ -2287,7 +2294,7 @@
       <c r="J20" s="31"/>
       <c r="M20" s="31"/>
     </row>
-    <row r="21" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>12</v>
       </c>
@@ -2307,7 +2314,7 @@
       <c r="J21" s="31"/>
       <c r="M21" s="31"/>
     </row>
-    <row r="22" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
         <v>14</v>
       </c>
@@ -2327,7 +2334,7 @@
       <c r="J22" s="31"/>
       <c r="M22" s="31"/>
     </row>
-    <row r="23" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
@@ -2347,7 +2354,7 @@
       <c r="J23" s="31"/>
       <c r="M23" s="31"/>
     </row>
-    <row r="24" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="2"/>
@@ -2361,7 +2368,7 @@
       <c r="J24" s="31"/>
       <c r="M24" s="31"/>
     </row>
-    <row r="25" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="s">
         <v>61</v>
       </c>
@@ -2376,7 +2383,7 @@
       <c r="M25" s="31"/>
       <c r="P25" s="31"/>
     </row>
-    <row r="26" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
@@ -2395,7 +2402,7 @@
       <c r="I26" s="31"/>
       <c r="L26" s="31"/>
     </row>
-    <row r="27" spans="1:16" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>62</v>
       </c>
@@ -2415,7 +2422,7 @@
       <c r="I27" s="31"/>
       <c r="L27" s="31"/>
     </row>
-    <row r="28" spans="1:16" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>64</v>
       </c>
@@ -2435,7 +2442,7 @@
       <c r="I28" s="31"/>
       <c r="L28" s="31"/>
     </row>
-    <row r="29" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>66</v>
       </c>
@@ -2455,7 +2462,7 @@
       <c r="I29" s="31"/>
       <c r="L29" s="31"/>
     </row>
-    <row r="30" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>68</v>
       </c>
@@ -2475,7 +2482,7 @@
       <c r="I30" s="31"/>
       <c r="L30" s="31"/>
     </row>
-    <row r="31" spans="1:16" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>70</v>
       </c>
@@ -2495,7 +2502,7 @@
       <c r="I31" s="31"/>
       <c r="L31" s="31"/>
     </row>
-    <row r="32" spans="1:16" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>71</v>
       </c>
@@ -2515,7 +2522,7 @@
       <c r="I32" s="31"/>
       <c r="L32" s="31"/>
     </row>
-    <row r="33" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>72</v>
       </c>
@@ -2535,7 +2542,7 @@
       <c r="I33" s="31"/>
       <c r="L33" s="31"/>
     </row>
-    <row r="34" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="42"/>
       <c r="B34" s="42"/>
       <c r="C34" s="30"/>
@@ -2549,7 +2556,7 @@
       <c r="K34" s="31"/>
       <c r="N34" s="31"/>
     </row>
-    <row r="35" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="61" t="s">
         <v>74</v>
       </c>
@@ -2564,7 +2571,7 @@
       <c r="M35" s="31"/>
       <c r="P35" s="31"/>
     </row>
-    <row r="36" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>7</v>
       </c>
@@ -2583,7 +2590,7 @@
       <c r="H36" s="31"/>
       <c r="K36" s="31"/>
     </row>
-    <row r="37" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>18</v>
       </c>
@@ -2603,7 +2610,7 @@
       <c r="H37" s="31"/>
       <c r="K37" s="31"/>
     </row>
-    <row r="38" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>19</v>
       </c>
@@ -2623,7 +2630,7 @@
       <c r="H38" s="31"/>
       <c r="K38" s="31"/>
     </row>
-    <row r="39" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>20</v>
       </c>
@@ -2643,7 +2650,7 @@
       <c r="H39" s="31"/>
       <c r="K39" s="31"/>
     </row>
-    <row r="40" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>21</v>
       </c>
@@ -2663,7 +2670,7 @@
       <c r="H40" s="31"/>
       <c r="K40" s="31"/>
     </row>
-    <row r="41" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>22</v>
       </c>
@@ -2683,7 +2690,7 @@
       <c r="H41" s="31"/>
       <c r="K41" s="31"/>
     </row>
-    <row r="42" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>23</v>
       </c>
@@ -2702,7 +2709,7 @@
       </c>
       <c r="I42" s="31"/>
     </row>
-    <row r="43" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>24</v>
       </c>
@@ -2723,7 +2730,7 @@
       <c r="I43" s="31"/>
       <c r="L43" s="31"/>
     </row>
-    <row r="44" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>25</v>
       </c>
@@ -2743,7 +2750,7 @@
       <c r="J44" s="31"/>
       <c r="M44" s="31"/>
     </row>
-    <row r="45" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2756,7 +2763,7 @@
       </c>
       <c r="V45" s="31"/>
     </row>
-    <row r="46" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2765,7 +2772,7 @@
       <c r="I46" s="2"/>
       <c r="Q46" s="31"/>
     </row>
-    <row r="47" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D47" s="47" t="s">
         <v>26</v>
       </c>
@@ -2775,10 +2782,10 @@
       </c>
       <c r="L47" s="31"/>
     </row>
-    <row r="48" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="L48" s="31"/>
     </row>
-    <row r="49" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" s="49" t="s">
         <v>76</v>
       </c>
@@ -2788,7 +2795,7 @@
       </c>
       <c r="L49" s="31"/>
     </row>
-    <row r="50" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="49" t="s">
         <v>155</v>
       </c>
@@ -2798,7 +2805,7 @@
       </c>
       <c r="L50" s="31"/>
     </row>
-    <row r="51" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="49" t="s">
         <v>77</v>
       </c>
@@ -2807,7 +2814,7 @@
       </c>
       <c r="L51" s="31"/>
     </row>
-    <row r="52" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="51" t="s">
         <v>27</v>
       </c>
@@ -2818,11 +2825,11 @@
       <c r="I52" s="31"/>
       <c r="Q52" s="31"/>
     </row>
-    <row r="53" spans="1:17" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="J53" s="31"/>
       <c r="K53" s="31"/>
     </row>
-    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="49" t="s">
         <v>28</v>
       </c>
@@ -2836,7 +2843,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>31</v>
       </c>
@@ -2851,989 +2858,989 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="53"/>
     </row>
-    <row r="57" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="54"/>
       <c r="B57" s="54"/>
     </row>
-    <row r="58" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="54"/>
       <c r="B58" s="54"/>
     </row>
-    <row r="59" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="54"/>
       <c r="B59" s="54"/>
     </row>
-    <row r="60" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1004" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1006" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1007" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1008" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1009" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1010" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1011" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1012" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1013" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1014" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1015" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1017" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1018" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1020" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1021" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1023" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1024" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1025" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1026" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1027" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="992" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="993" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="994" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1020" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1021" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1022" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1023" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1024" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1025" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1026" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1027" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A17:E17"/>

</xml_diff>